<commit_message>
transformation du site en mode gdm
</commit_message>
<xml_diff>
--- a/assets/docs/Tableau de synthèse.xlsx
+++ b/assets/docs/Tableau de synthèse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrateur1\Documents\PorfolioSaintJo\assets\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF57ABDC-049D-47F5-BB89-0C273F87B5DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259CC02E-9B21-4CA7-97F8-BE3A7BDC5479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tableau de synthèse Épreuve E5" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E5'!$A$1:$H$53</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E5'!$A$1:$H$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -145,101 +145,27 @@
     <t>Configuration de serveurs (SRFIC, SSR), déploiement PXE</t>
   </si>
   <si>
-    <t>Intervention câblage fibre (Culoz)</t>
-  </si>
-  <si>
-    <t>Résolution de problèmes liés aux lecteurs de carte V1/V2</t>
-  </si>
-  <si>
     <t>Gestion des mails (Dovecot, spam)</t>
   </si>
   <si>
     <t>Mise en place de serveurs (SAV, SMS).</t>
   </si>
   <si>
-    <t>Utilisation de Python pour automatisation.</t>
-  </si>
-  <si>
-    <t>Découverte d’outils métiers (Check Mon Compte).</t>
-  </si>
-  <si>
     <t>Vérification des droits ACL sur les partages de fichiers</t>
   </si>
   <si>
     <t>Inventaire de serveurs; comptage des disques durs; saisis d'ordinateur</t>
-  </si>
-  <si>
-    <t>Mise en place de RAID 1 et RAID 5 (sur un serveur fic et kvm)</t>
   </si>
   <si>
     <t xml:space="preserve">Hotline (problèmes LRPGN, certificats, Thunderbird, impressions ect..).
 </t>
   </si>
   <si>
-    <t>Installation d’un AD et création d’un utilisateur dans l’AD</t>
-  </si>
-  <si>
-    <t>Mise en place d’un GPO sous Windows Server</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mise en place d’un RAID 1 sous Linux avec mdadm
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mise en place d’une sauvegarde via Veeam
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Vérification du fonctionnement d’une table de routage dans CMD
-</t>
-  </si>
-  <si>
-    <t>Ajout d’un utilisateur dans un domaine Windows Server</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Création d’un groupe et des dossiers de partage
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Effectuer un mappage réseau
-</t>
-  </si>
-  <si>
-    <t>Installation de différents OS (Debian, Windows Server)</t>
-  </si>
-  <si>
-    <t>Installation d’un Windows 11 classique sur VirtualBox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Installation d’un DualBoot
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Installation d’un serveur de fichiers
-</t>
-  </si>
-  <si>
     <t>Installation et configuration de pfSense</t>
-  </si>
-  <si>
-    <t>Configuration d’un routeur entre deux réseaux</t>
-  </si>
-  <si>
-    <t>Configuration d’une borne Wi-Fi</t>
-  </si>
-  <si>
-    <t>Configuration d’un serveur DNS</t>
-  </si>
-  <si>
-    <t>Installation d’un serveur DHCP sous Debian/Windows Server</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Configuration d’une IP fixe sous Debian
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mise en place du TSE sous Windows Server
-</t>
   </si>
   <si>
     <t xml:space="preserve">Configuration d’IIS 10 (serveur web)
@@ -250,26 +176,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Configuration d’une base de données MySQL avec PhpMyAdmin
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mise en place d’un serveur GLPI
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Installation de NocoDB
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Configuration de VLAN Access et VLAN Trunk
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Export d’une VM VirtualBox sur Proxmox
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Réalisation en cours de formation
 </t>
   </si>
@@ -280,10 +190,24 @@
     <t>X</t>
   </si>
   <si>
-    <t>Déploiement de 25 Windows 10 (pour formation Ntech).</t>
-  </si>
-  <si>
     <t>Installation de PC Ubiquity (OS, chiffrement,VPN,cryptage).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuration de VLAN Access et VLAN Trunk(via interface)
+</t>
+  </si>
+  <si>
+    <t>Installation de différents OS (Debian, Windows Server), dualboot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Securisation de donnée sous Linux avec mdadm
+</t>
+  </si>
+  <si>
+    <t>Installation d’un AD,création d’un utilisateur, mise en place d'une GPO,partage de fichiers</t>
+  </si>
+  <si>
+    <t>Installation d’un serveur DHCP sous Debian/Windows Server/Pfense</t>
   </si>
 </sst>
 </file>
@@ -709,7 +633,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -735,12 +659,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -771,9 +689,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -796,45 +753,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1214,10 +1132,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ99"/>
+  <dimension ref="A1:AQ79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="40" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1230,83 +1148,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="21"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="28" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="29"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="40"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="27"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="42"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="32"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="28" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1329,24 +1247,24 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="34"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="12" t="s">
+      <c r="A7" s="23"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="11" t="s">
         <v>14</v>
       </c>
       <c r="I7"/>
@@ -1386,16 +1304,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="27"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1434,18 +1352,18 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="18" t="s">
-        <v>67</v>
+        <v>33</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="16" t="s">
+        <v>41</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
@@ -1478,17 +1396,17 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18"/>
+      <c r="C10" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="16"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1523,14 +1441,14 @@
         <v>25</v>
       </c>
       <c r="B11" s="5"/>
-      <c r="C11" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
+      <c r="C11" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="16"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1565,19 +1483,19 @@
         <v>26</v>
       </c>
       <c r="B12" s="5"/>
-      <c r="C12" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18" t="s">
-        <v>68</v>
+      <c r="C12" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="16" t="s">
+        <v>42</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>
@@ -1613,16 +1531,16 @@
         <v>27</v>
       </c>
       <c r="B13" s="5"/>
-      <c r="C13" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H13" s="18"/>
+      <c r="C13" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="16"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1654,19 +1572,21 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H14" s="18"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>42</v>
+      </c>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1698,20 +1618,20 @@
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H15" s="18" t="s">
-        <v>68</v>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="16" t="s">
+        <v>42</v>
       </c>
       <c r="I15"/>
       <c r="J15"/>
@@ -1744,21 +1664,19 @@
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B16" s="5"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="18" t="s">
-        <v>68</v>
-      </c>
+      <c r="C16" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="16"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1790,19 +1708,21 @@
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17" s="5"/>
-      <c r="C17" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H17" s="18"/>
+      <c r="C17" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="16"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1834,19 +1754,19 @@
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="5"/>
-      <c r="C18" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H18" s="18"/>
+      <c r="C18" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" s="16"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1878,17 +1798,19 @@
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B19" s="5"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="18"/>
+      <c r="C19" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" s="16"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1916,25 +1838,8 @@
       <c r="AG19"/>
       <c r="AH19"/>
       <c r="AI19"/>
-      <c r="AJ19"/>
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H20" s="18"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -1962,22 +1867,19 @@
       <c r="AG20"/>
       <c r="AH20"/>
       <c r="AI20"/>
+      <c r="AJ20"/>
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H21" s="18"/>
+      <c r="A21" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -1998,30 +1900,22 @@
       <c r="Z21"/>
       <c r="AA21"/>
       <c r="AB21"/>
-      <c r="AC21"/>
-      <c r="AD21"/>
-      <c r="AE21"/>
-      <c r="AF21"/>
-      <c r="AG21"/>
-      <c r="AH21"/>
-      <c r="AI21"/>
-      <c r="AJ21"/>
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H22" s="18"/>
+        <v>47</v>
+      </c>
+      <c r="B22" s="14"/>
+      <c r="C22" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="15"/>
+      <c r="H22" s="16"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -2050,22 +1944,29 @@
       <c r="AH22"/>
       <c r="AI22"/>
       <c r="AJ22"/>
+      <c r="AK22"/>
+      <c r="AL22"/>
+      <c r="AM22"/>
+      <c r="AN22"/>
+      <c r="AO22"/>
+      <c r="AP22"/>
+      <c r="AQ22"/>
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H23" s="18"/>
+        <v>46</v>
+      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="15"/>
+      <c r="H23" s="16"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -2094,24 +1995,29 @@
       <c r="AH23"/>
       <c r="AI23"/>
       <c r="AJ23"/>
+      <c r="AK23"/>
+      <c r="AL23"/>
+      <c r="AM23"/>
+      <c r="AN23"/>
+      <c r="AO23"/>
+      <c r="AP23"/>
+      <c r="AQ23"/>
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H24" s="18" t="s">
-        <v>68</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="15"/>
+      <c r="H24" s="16"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -2132,20 +2038,37 @@
       <c r="Z24"/>
       <c r="AA24"/>
       <c r="AB24"/>
+      <c r="AC24"/>
+      <c r="AD24"/>
+      <c r="AE24"/>
+      <c r="AF24"/>
+      <c r="AG24"/>
+      <c r="AH24"/>
+      <c r="AI24"/>
+      <c r="AJ24"/>
+      <c r="AK24"/>
+      <c r="AL24"/>
+      <c r="AM24"/>
+      <c r="AN24"/>
+      <c r="AO24"/>
+      <c r="AP24"/>
+      <c r="AQ24"/>
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="17"/>
+      <c r="A25" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15" t="s">
+        <v>42</v>
+      </c>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
+      <c r="F25" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="G25" s="17"/>
-      <c r="H25" s="18" t="s">
-        <v>68</v>
-      </c>
+      <c r="H25" s="18"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2174,18 +2097,29 @@
       <c r="AH25"/>
       <c r="AI25"/>
       <c r="AJ25"/>
+      <c r="AK25"/>
+      <c r="AL25"/>
+      <c r="AM25"/>
+      <c r="AN25"/>
+      <c r="AO25"/>
+      <c r="AP25"/>
+      <c r="AQ25"/>
     </row>
     <row r="26" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="32"/>
+      <c r="A26" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="14"/>
+      <c r="C26" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="17"/>
+      <c r="H26" s="18"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2222,15 +2156,21 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="10"/>
+    <row r="27" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="17"/>
+      <c r="H27" s="18"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2268,17 +2208,19 @@
       <c r="AQ27"/>
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="17" t="s">
-        <v>68</v>
+      <c r="A28" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="14"/>
+      <c r="C28" s="15" t="s">
+        <v>42</v>
       </c>
       <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
+      <c r="E28" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="F28" s="17" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="18"/>
@@ -2319,17 +2261,19 @@
       <c r="AQ28"/>
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="17" t="s">
-        <v>68</v>
+      <c r="A29" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="14"/>
+      <c r="C29" s="15" t="s">
+        <v>42</v>
       </c>
       <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
+      <c r="E29" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="F29" s="17" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="18"/>
@@ -2370,17 +2314,17 @@
       <c r="AQ29"/>
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="17" t="s">
-        <v>68</v>
+      <c r="A30" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="14"/>
+      <c r="C30" s="15" t="s">
+        <v>42</v>
       </c>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
       <c r="F30" s="17" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="G30" s="17"/>
       <c r="H30" s="18"/>
@@ -2421,17 +2365,17 @@
       <c r="AQ30"/>
     </row>
     <row r="31" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="17" t="s">
-        <v>68</v>
+      <c r="A31" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="14"/>
+      <c r="C31" s="15" t="s">
+        <v>42</v>
       </c>
       <c r="D31" s="17"/>
       <c r="E31" s="17"/>
       <c r="F31" s="17" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="G31" s="17"/>
       <c r="H31" s="18"/>
@@ -2472,18 +2416,14 @@
       <c r="AQ31"/>
     </row>
     <row r="32" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="16"/>
-      <c r="C32" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="18"/>
+      <c r="A32"/>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
@@ -2521,20 +2461,14 @@
       <c r="AQ32"/>
     </row>
     <row r="33" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" s="16"/>
-      <c r="C33" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G33" s="19"/>
-      <c r="H33" s="20"/>
+      <c r="A33"/>
+      <c r="B33"/>
+      <c r="C33" s="1"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
@@ -2571,1104 +2505,92 @@
       <c r="AP33"/>
       <c r="AQ33"/>
     </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" s="16"/>
-      <c r="C34" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G34" s="19"/>
-      <c r="H34" s="20"/>
-      <c r="I34"/>
-      <c r="J34"/>
-      <c r="K34"/>
-      <c r="L34"/>
-      <c r="M34"/>
-      <c r="N34"/>
-      <c r="O34"/>
-      <c r="P34"/>
-      <c r="Q34"/>
-      <c r="R34"/>
-      <c r="S34"/>
-      <c r="T34"/>
-      <c r="U34"/>
-      <c r="V34"/>
-      <c r="W34"/>
-      <c r="X34"/>
-      <c r="Y34"/>
-      <c r="Z34"/>
-      <c r="AA34"/>
-      <c r="AB34"/>
-      <c r="AC34"/>
-      <c r="AD34"/>
-      <c r="AE34"/>
-      <c r="AF34"/>
-      <c r="AG34"/>
-      <c r="AH34"/>
-      <c r="AI34"/>
-      <c r="AJ34"/>
-      <c r="AK34"/>
-      <c r="AL34"/>
-      <c r="AM34"/>
-      <c r="AN34"/>
-      <c r="AO34"/>
-      <c r="AP34"/>
-      <c r="AQ34"/>
-    </row>
-    <row r="35" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" s="16"/>
-      <c r="C35" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G35" s="19"/>
-      <c r="H35" s="20"/>
-      <c r="I35"/>
-      <c r="J35"/>
-      <c r="K35"/>
-      <c r="L35"/>
-      <c r="M35"/>
-      <c r="N35"/>
-      <c r="O35"/>
-      <c r="P35"/>
-      <c r="Q35"/>
-      <c r="R35"/>
-      <c r="S35"/>
-      <c r="T35"/>
-      <c r="U35"/>
-      <c r="V35"/>
-      <c r="W35"/>
-      <c r="X35"/>
-      <c r="Y35"/>
-      <c r="Z35"/>
-      <c r="AA35"/>
-      <c r="AB35"/>
-      <c r="AC35"/>
-      <c r="AD35"/>
-      <c r="AE35"/>
-      <c r="AF35"/>
-      <c r="AG35"/>
-      <c r="AH35"/>
-      <c r="AI35"/>
-      <c r="AJ35"/>
-      <c r="AK35"/>
-      <c r="AL35"/>
-      <c r="AM35"/>
-      <c r="AN35"/>
-      <c r="AO35"/>
-      <c r="AP35"/>
-      <c r="AQ35"/>
-    </row>
-    <row r="36" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="16"/>
-      <c r="C36" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G36" s="19"/>
-      <c r="H36" s="20"/>
-      <c r="I36"/>
-      <c r="J36"/>
-      <c r="K36"/>
-      <c r="L36"/>
-      <c r="M36"/>
-      <c r="N36"/>
-      <c r="O36"/>
-      <c r="P36"/>
-      <c r="Q36"/>
-      <c r="R36"/>
-      <c r="S36"/>
-      <c r="T36"/>
-      <c r="U36"/>
-      <c r="V36"/>
-      <c r="W36"/>
-      <c r="X36"/>
-      <c r="Y36"/>
-      <c r="Z36"/>
-      <c r="AA36"/>
-      <c r="AB36"/>
-      <c r="AC36"/>
-      <c r="AD36"/>
-      <c r="AE36"/>
-      <c r="AF36"/>
-      <c r="AG36"/>
-      <c r="AH36"/>
-      <c r="AI36"/>
-      <c r="AJ36"/>
-      <c r="AK36"/>
-      <c r="AL36"/>
-      <c r="AM36"/>
-      <c r="AN36"/>
-      <c r="AO36"/>
-      <c r="AP36"/>
-      <c r="AQ36"/>
-    </row>
-    <row r="37" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" s="16"/>
-      <c r="C37" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G37" s="19"/>
-      <c r="H37" s="20"/>
-      <c r="I37"/>
-      <c r="J37"/>
-      <c r="K37"/>
-      <c r="L37"/>
-      <c r="M37"/>
-      <c r="N37"/>
-      <c r="O37"/>
-      <c r="P37"/>
-      <c r="Q37"/>
-      <c r="R37"/>
-      <c r="S37"/>
-      <c r="T37"/>
-      <c r="U37"/>
-      <c r="V37"/>
-      <c r="W37"/>
-      <c r="X37"/>
-      <c r="Y37"/>
-      <c r="Z37"/>
-      <c r="AA37"/>
-      <c r="AB37"/>
-      <c r="AC37"/>
-      <c r="AD37"/>
-      <c r="AE37"/>
-      <c r="AF37"/>
-      <c r="AG37"/>
-      <c r="AH37"/>
-      <c r="AI37"/>
-      <c r="AJ37"/>
-      <c r="AK37"/>
-      <c r="AL37"/>
-      <c r="AM37"/>
-      <c r="AN37"/>
-      <c r="AO37"/>
-      <c r="AP37"/>
-      <c r="AQ37"/>
-    </row>
-    <row r="38" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" s="16"/>
-      <c r="C38" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G38" s="19"/>
-      <c r="H38" s="20"/>
-      <c r="I38"/>
-      <c r="J38"/>
-      <c r="K38"/>
-      <c r="L38"/>
-      <c r="M38"/>
-      <c r="N38"/>
-      <c r="O38"/>
-      <c r="P38"/>
-      <c r="Q38"/>
-      <c r="R38"/>
-      <c r="S38"/>
-      <c r="T38"/>
-      <c r="U38"/>
-      <c r="V38"/>
-      <c r="W38"/>
-      <c r="X38"/>
-      <c r="Y38"/>
-      <c r="Z38"/>
-      <c r="AA38"/>
-      <c r="AB38"/>
-      <c r="AC38"/>
-      <c r="AD38"/>
-      <c r="AE38"/>
-      <c r="AF38"/>
-      <c r="AG38"/>
-      <c r="AH38"/>
-      <c r="AI38"/>
-      <c r="AJ38"/>
-      <c r="AK38"/>
-      <c r="AL38"/>
-      <c r="AM38"/>
-      <c r="AN38"/>
-      <c r="AO38"/>
-      <c r="AP38"/>
-      <c r="AQ38"/>
-    </row>
-    <row r="39" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B39" s="16"/>
-      <c r="C39" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G39" s="19"/>
-      <c r="H39" s="20"/>
-      <c r="I39"/>
-      <c r="J39"/>
-      <c r="K39"/>
-      <c r="L39"/>
-      <c r="M39"/>
-      <c r="N39"/>
-      <c r="O39"/>
-      <c r="P39"/>
-      <c r="Q39"/>
-      <c r="R39"/>
-      <c r="S39"/>
-      <c r="T39"/>
-      <c r="U39"/>
-      <c r="V39"/>
-      <c r="W39"/>
-      <c r="X39"/>
-      <c r="Y39"/>
-      <c r="Z39"/>
-      <c r="AA39"/>
-      <c r="AB39"/>
-      <c r="AC39"/>
-      <c r="AD39"/>
-      <c r="AE39"/>
-      <c r="AF39"/>
-      <c r="AG39"/>
-      <c r="AH39"/>
-      <c r="AI39"/>
-      <c r="AJ39"/>
-      <c r="AK39"/>
-      <c r="AL39"/>
-      <c r="AM39"/>
-      <c r="AN39"/>
-      <c r="AO39"/>
-      <c r="AP39"/>
-      <c r="AQ39"/>
-    </row>
-    <row r="40" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" s="16"/>
-      <c r="C40" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G40" s="19"/>
-      <c r="H40" s="20"/>
-      <c r="I40"/>
-      <c r="J40"/>
-      <c r="K40"/>
-      <c r="L40"/>
-      <c r="M40"/>
-      <c r="N40"/>
-      <c r="O40"/>
-      <c r="P40"/>
-      <c r="Q40"/>
-      <c r="R40"/>
-      <c r="S40"/>
-      <c r="T40"/>
-      <c r="U40"/>
-      <c r="V40"/>
-      <c r="W40"/>
-      <c r="X40"/>
-      <c r="Y40"/>
-      <c r="Z40"/>
-      <c r="AA40"/>
-      <c r="AB40"/>
-      <c r="AC40"/>
-      <c r="AD40"/>
-      <c r="AE40"/>
-      <c r="AF40"/>
-      <c r="AG40"/>
-      <c r="AH40"/>
-      <c r="AI40"/>
-      <c r="AJ40"/>
-      <c r="AK40"/>
-      <c r="AL40"/>
-      <c r="AM40"/>
-      <c r="AN40"/>
-      <c r="AO40"/>
-      <c r="AP40"/>
-      <c r="AQ40"/>
-    </row>
-    <row r="41" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" s="16"/>
-      <c r="C41" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G41" s="19"/>
-      <c r="H41" s="20"/>
-      <c r="I41"/>
-      <c r="J41"/>
-      <c r="K41"/>
-      <c r="L41"/>
-      <c r="M41"/>
-      <c r="N41"/>
-      <c r="O41"/>
-      <c r="P41"/>
-      <c r="Q41"/>
-      <c r="R41"/>
-      <c r="S41"/>
-      <c r="T41"/>
-      <c r="U41"/>
-      <c r="V41"/>
-      <c r="W41"/>
-      <c r="X41"/>
-      <c r="Y41"/>
-      <c r="Z41"/>
-      <c r="AA41"/>
-      <c r="AB41"/>
-      <c r="AC41"/>
-      <c r="AD41"/>
-      <c r="AE41"/>
-      <c r="AF41"/>
-      <c r="AG41"/>
-      <c r="AH41"/>
-      <c r="AI41"/>
-      <c r="AJ41"/>
-      <c r="AK41"/>
-      <c r="AL41"/>
-      <c r="AM41"/>
-      <c r="AN41"/>
-      <c r="AO41"/>
-      <c r="AP41"/>
-      <c r="AQ41"/>
-    </row>
-    <row r="42" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" s="16"/>
-      <c r="C42" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G42" s="19"/>
-      <c r="H42" s="20"/>
-      <c r="I42"/>
-      <c r="J42"/>
-      <c r="K42"/>
-      <c r="L42"/>
-      <c r="M42"/>
-      <c r="N42"/>
-      <c r="O42"/>
-      <c r="P42"/>
-      <c r="Q42"/>
-      <c r="R42"/>
-      <c r="S42"/>
-      <c r="T42"/>
-      <c r="U42"/>
-      <c r="V42"/>
-      <c r="W42"/>
-      <c r="X42"/>
-      <c r="Y42"/>
-      <c r="Z42"/>
-      <c r="AA42"/>
-      <c r="AB42"/>
-      <c r="AC42"/>
-      <c r="AD42"/>
-      <c r="AE42"/>
-      <c r="AF42"/>
-      <c r="AG42"/>
-      <c r="AH42"/>
-      <c r="AI42"/>
-      <c r="AJ42"/>
-      <c r="AK42"/>
-      <c r="AL42"/>
-      <c r="AM42"/>
-      <c r="AN42"/>
-      <c r="AO42"/>
-      <c r="AP42"/>
-      <c r="AQ42"/>
-    </row>
-    <row r="43" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G43" s="19"/>
-      <c r="H43" s="20"/>
-      <c r="I43"/>
-      <c r="J43"/>
-      <c r="K43"/>
-      <c r="L43"/>
-      <c r="M43"/>
-      <c r="N43"/>
-      <c r="O43"/>
-      <c r="P43"/>
-      <c r="Q43"/>
-      <c r="R43"/>
-      <c r="S43"/>
-      <c r="T43"/>
-      <c r="U43"/>
-      <c r="V43"/>
-      <c r="W43"/>
-      <c r="X43"/>
-      <c r="Y43"/>
-      <c r="Z43"/>
-      <c r="AA43"/>
-      <c r="AB43"/>
-      <c r="AC43"/>
-      <c r="AD43"/>
-      <c r="AE43"/>
-      <c r="AF43"/>
-      <c r="AG43"/>
-      <c r="AH43"/>
-      <c r="AI43"/>
-      <c r="AJ43"/>
-      <c r="AK43"/>
-      <c r="AL43"/>
-      <c r="AM43"/>
-      <c r="AN43"/>
-      <c r="AO43"/>
-      <c r="AP43"/>
-      <c r="AQ43"/>
-    </row>
-    <row r="44" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="B44" s="16"/>
-      <c r="C44" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G44" s="19"/>
-      <c r="H44" s="20"/>
-      <c r="I44"/>
-      <c r="J44"/>
-      <c r="K44"/>
-      <c r="L44"/>
-      <c r="M44"/>
-      <c r="N44"/>
-      <c r="O44"/>
-      <c r="P44"/>
-      <c r="Q44"/>
-      <c r="R44"/>
-      <c r="S44"/>
-      <c r="T44"/>
-      <c r="U44"/>
-      <c r="V44"/>
-      <c r="W44"/>
-      <c r="X44"/>
-      <c r="Y44"/>
-      <c r="Z44"/>
-      <c r="AA44"/>
-      <c r="AB44"/>
-      <c r="AC44"/>
-      <c r="AD44"/>
-      <c r="AE44"/>
-      <c r="AF44"/>
-      <c r="AG44"/>
-      <c r="AH44"/>
-      <c r="AI44"/>
-      <c r="AJ44"/>
-      <c r="AK44"/>
-      <c r="AL44"/>
-      <c r="AM44"/>
-      <c r="AN44"/>
-      <c r="AO44"/>
-      <c r="AP44"/>
-      <c r="AQ44"/>
-    </row>
-    <row r="45" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B45" s="16"/>
-      <c r="C45" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G45" s="19"/>
-      <c r="H45" s="20"/>
-      <c r="I45"/>
-      <c r="J45"/>
-      <c r="K45"/>
-      <c r="L45"/>
-      <c r="M45"/>
-      <c r="N45"/>
-      <c r="O45"/>
-      <c r="P45"/>
-      <c r="Q45"/>
-      <c r="R45"/>
-      <c r="S45"/>
-      <c r="T45"/>
-      <c r="U45"/>
-      <c r="V45"/>
-      <c r="W45"/>
-      <c r="X45"/>
-      <c r="Y45"/>
-      <c r="Z45"/>
-      <c r="AA45"/>
-      <c r="AB45"/>
-      <c r="AC45"/>
-      <c r="AD45"/>
-      <c r="AE45"/>
-      <c r="AF45"/>
-      <c r="AG45"/>
-      <c r="AH45"/>
-      <c r="AI45"/>
-      <c r="AJ45"/>
-      <c r="AK45"/>
-      <c r="AL45"/>
-      <c r="AM45"/>
-      <c r="AN45"/>
-      <c r="AO45"/>
-      <c r="AP45"/>
-      <c r="AQ45"/>
-    </row>
-    <row r="46" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B46" s="16"/>
-      <c r="C46" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G46" s="19"/>
-      <c r="H46" s="20"/>
-      <c r="I46"/>
-      <c r="J46"/>
-      <c r="K46"/>
-      <c r="L46"/>
-      <c r="M46"/>
-      <c r="N46"/>
-      <c r="O46"/>
-      <c r="P46"/>
-      <c r="Q46"/>
-      <c r="R46"/>
-      <c r="S46"/>
-      <c r="T46"/>
-      <c r="U46"/>
-      <c r="V46"/>
-      <c r="W46"/>
-      <c r="X46"/>
-      <c r="Y46"/>
-      <c r="Z46"/>
-      <c r="AA46"/>
-      <c r="AB46"/>
-      <c r="AC46"/>
-      <c r="AD46"/>
-      <c r="AE46"/>
-      <c r="AF46"/>
-      <c r="AG46"/>
-      <c r="AH46"/>
-      <c r="AI46"/>
-      <c r="AJ46"/>
-      <c r="AK46"/>
-      <c r="AL46"/>
-      <c r="AM46"/>
-      <c r="AN46"/>
-      <c r="AO46"/>
-      <c r="AP46"/>
-      <c r="AQ46"/>
-    </row>
-    <row r="47" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47" s="16"/>
-      <c r="C47" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="F47" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G47" s="19"/>
-      <c r="H47" s="20"/>
-      <c r="I47"/>
-      <c r="J47"/>
-      <c r="K47"/>
-      <c r="L47"/>
-      <c r="M47"/>
-      <c r="N47"/>
-      <c r="O47"/>
-      <c r="P47"/>
-      <c r="Q47"/>
-      <c r="R47"/>
-      <c r="S47"/>
-      <c r="T47"/>
-      <c r="U47"/>
-      <c r="V47"/>
-      <c r="W47"/>
-      <c r="X47"/>
-      <c r="Y47"/>
-      <c r="Z47"/>
-      <c r="AA47"/>
-      <c r="AB47"/>
-      <c r="AC47"/>
-      <c r="AD47"/>
-      <c r="AE47"/>
-      <c r="AF47"/>
-      <c r="AG47"/>
-      <c r="AH47"/>
-      <c r="AI47"/>
-      <c r="AJ47"/>
-      <c r="AK47"/>
-      <c r="AL47"/>
-      <c r="AM47"/>
-      <c r="AN47"/>
-      <c r="AO47"/>
-      <c r="AP47"/>
-      <c r="AQ47"/>
-    </row>
-    <row r="48" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B48" s="16"/>
-      <c r="C48" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="F48" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G48" s="19"/>
-      <c r="H48" s="20"/>
-      <c r="I48"/>
-      <c r="J48"/>
-      <c r="K48"/>
-      <c r="L48"/>
-      <c r="M48"/>
-      <c r="N48"/>
-      <c r="O48"/>
-      <c r="P48"/>
-      <c r="Q48"/>
-      <c r="R48"/>
-      <c r="S48"/>
-      <c r="T48"/>
-      <c r="U48"/>
-      <c r="V48"/>
-      <c r="W48"/>
-      <c r="X48"/>
-      <c r="Y48"/>
-      <c r="Z48"/>
-      <c r="AA48"/>
-      <c r="AB48"/>
-      <c r="AC48"/>
-      <c r="AD48"/>
-      <c r="AE48"/>
-      <c r="AF48"/>
-      <c r="AG48"/>
-      <c r="AH48"/>
-      <c r="AI48"/>
-      <c r="AJ48"/>
-      <c r="AK48"/>
-      <c r="AL48"/>
-      <c r="AM48"/>
-      <c r="AN48"/>
-      <c r="AO48"/>
-      <c r="AP48"/>
-      <c r="AQ48"/>
-    </row>
-    <row r="49" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B49" s="16"/>
-      <c r="C49" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="F49" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G49" s="19"/>
-      <c r="H49" s="20"/>
-      <c r="I49"/>
-      <c r="J49"/>
-      <c r="K49"/>
-      <c r="L49"/>
-      <c r="M49"/>
-      <c r="N49"/>
-      <c r="O49"/>
-      <c r="P49"/>
-      <c r="Q49"/>
-      <c r="R49"/>
-      <c r="S49"/>
-      <c r="T49"/>
-      <c r="U49"/>
-      <c r="V49"/>
-      <c r="W49"/>
-      <c r="X49"/>
-      <c r="Y49"/>
-      <c r="Z49"/>
-      <c r="AA49"/>
-      <c r="AB49"/>
-      <c r="AC49"/>
-      <c r="AD49"/>
-      <c r="AE49"/>
-      <c r="AF49"/>
-      <c r="AG49"/>
-      <c r="AH49"/>
-      <c r="AI49"/>
-      <c r="AJ49"/>
-      <c r="AK49"/>
-      <c r="AL49"/>
-      <c r="AM49"/>
-      <c r="AN49"/>
-      <c r="AO49"/>
-      <c r="AP49"/>
-      <c r="AQ49"/>
-    </row>
-    <row r="50" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B50" s="16"/>
-      <c r="C50" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G50" s="19"/>
-      <c r="H50" s="20"/>
-      <c r="I50"/>
-      <c r="J50"/>
-      <c r="K50"/>
-      <c r="L50"/>
-      <c r="M50"/>
-      <c r="N50"/>
-      <c r="O50"/>
-      <c r="P50"/>
-      <c r="Q50"/>
-      <c r="R50"/>
-      <c r="S50"/>
-      <c r="T50"/>
-      <c r="U50"/>
-      <c r="V50"/>
-      <c r="W50"/>
-      <c r="X50"/>
-      <c r="Y50"/>
-      <c r="Z50"/>
-      <c r="AA50"/>
-      <c r="AB50"/>
-      <c r="AC50"/>
-      <c r="AD50"/>
-      <c r="AE50"/>
-      <c r="AF50"/>
-      <c r="AG50"/>
-      <c r="AH50"/>
-      <c r="AI50"/>
-      <c r="AJ50"/>
-      <c r="AK50"/>
-      <c r="AL50"/>
-      <c r="AM50"/>
-      <c r="AN50"/>
-      <c r="AO50"/>
-      <c r="AP50"/>
-      <c r="AQ50"/>
-    </row>
-    <row r="51" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B51" s="16"/>
-      <c r="C51" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="F51" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G51" s="19"/>
-      <c r="H51" s="20"/>
-      <c r="I51"/>
-      <c r="J51"/>
-      <c r="K51"/>
-      <c r="L51"/>
-      <c r="M51"/>
-      <c r="N51"/>
-      <c r="O51"/>
-      <c r="P51"/>
-      <c r="Q51"/>
-      <c r="R51"/>
-      <c r="S51"/>
-      <c r="T51"/>
-      <c r="U51"/>
-      <c r="V51"/>
-      <c r="W51"/>
-      <c r="X51"/>
-      <c r="Y51"/>
-      <c r="Z51"/>
-      <c r="AA51"/>
-      <c r="AB51"/>
-      <c r="AC51"/>
-      <c r="AD51"/>
-      <c r="AE51"/>
-      <c r="AF51"/>
-      <c r="AG51"/>
-      <c r="AH51"/>
-      <c r="AI51"/>
-      <c r="AJ51"/>
-      <c r="AK51"/>
-      <c r="AL51"/>
-      <c r="AM51"/>
-      <c r="AN51"/>
-      <c r="AO51"/>
-      <c r="AP51"/>
-      <c r="AQ51"/>
-    </row>
-    <row r="52" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" s="16"/>
-      <c r="C52" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G52" s="19"/>
-      <c r="H52" s="20"/>
-      <c r="I52"/>
-      <c r="J52"/>
-      <c r="K52"/>
-      <c r="L52"/>
-      <c r="M52"/>
-      <c r="N52"/>
-      <c r="O52"/>
-      <c r="P52"/>
-      <c r="Q52"/>
-      <c r="R52"/>
-      <c r="S52"/>
-      <c r="T52"/>
-      <c r="U52"/>
-      <c r="V52"/>
-      <c r="W52"/>
-      <c r="X52"/>
-      <c r="Y52"/>
-      <c r="Z52"/>
-      <c r="AA52"/>
-      <c r="AB52"/>
-      <c r="AC52"/>
-      <c r="AD52"/>
-      <c r="AE52"/>
-      <c r="AF52"/>
-      <c r="AG52"/>
-      <c r="AH52"/>
-      <c r="AI52"/>
-      <c r="AJ52"/>
-      <c r="AK52"/>
-      <c r="AL52"/>
-      <c r="AM52"/>
-      <c r="AN52"/>
-      <c r="AO52"/>
-      <c r="AP52"/>
-      <c r="AQ52"/>
-    </row>
-    <row r="53" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B53" s="16"/>
-      <c r="C53" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G53" s="19"/>
-      <c r="H53" s="20"/>
-      <c r="I53"/>
-      <c r="J53"/>
-      <c r="K53"/>
-      <c r="L53"/>
-      <c r="M53"/>
-      <c r="N53"/>
-      <c r="O53"/>
-      <c r="P53"/>
-      <c r="Q53"/>
-      <c r="R53"/>
-      <c r="S53"/>
-      <c r="T53"/>
-      <c r="U53"/>
-      <c r="V53"/>
-      <c r="W53"/>
-      <c r="X53"/>
-      <c r="Y53"/>
-      <c r="Z53"/>
-      <c r="AA53"/>
-      <c r="AB53"/>
-      <c r="AC53"/>
-      <c r="AD53"/>
-      <c r="AE53"/>
-      <c r="AF53"/>
-      <c r="AG53"/>
-      <c r="AH53"/>
-      <c r="AI53"/>
-      <c r="AJ53"/>
-      <c r="AK53"/>
-      <c r="AL53"/>
-      <c r="AM53"/>
-      <c r="AN53"/>
-      <c r="AO53"/>
-      <c r="AP53"/>
-      <c r="AQ53"/>
-    </row>
-    <row r="54" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C55" s="1"/>
-    </row>
-    <row r="56" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="98" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
-      <c r="E99" s="1"/>
-      <c r="F99" s="1"/>
-      <c r="G99" s="1"/>
-      <c r="H99" s="1"/>
+    <row r="34" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+    </row>
+    <row r="78" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+    </row>
+    <row r="79" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="A21:H21"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>